<commit_message>
Update database and main.py, replace old page files with emoji-named versions
</commit_message>
<xml_diff>
--- a/data_hiburan.xlsx
+++ b/data_hiburan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ewun\selira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6E73A5-3773-424F-A59E-30728AC18871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE552A09-1BD6-45ED-A077-2D95EEB28D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1714" uniqueCount="1007">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="1146">
   <si>
     <t>title</t>
   </si>
@@ -3044,13 +3044,705 @@
   </si>
   <si>
     <t>mm</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>narrator</t>
+  </si>
+  <si>
+    <t>goodreads_rating</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>cover</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>Indonesia X-Files</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/2F1DnzcmRg2b1K1ExJGRwS</t>
+  </si>
+  <si>
+    <t>Rahvayana: Aku Lala Padamu</t>
+  </si>
+  <si>
+    <t>Sujiwo Tejo</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/3rja5LL0jTl2QmDgrwNbjo</t>
+  </si>
+  <si>
+    <t>Rumah Tangga yang Bahagia</t>
+  </si>
+  <si>
+    <t>Leo Tolstoy</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/4wujUHwiQ4UeZmhUNk7H4J</t>
+  </si>
+  <si>
+    <t>Lelaki Tua dan Laut</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/719qnUT6Zm6m7IzQbbf4OO</t>
+  </si>
+  <si>
+    <t>Hari yang Sempurna untuk Kanguru</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/31c7kpXIOJUj7k8wcL8RMP</t>
+  </si>
+  <si>
+    <t>Pangeran Cilik</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/2EK3MJF4bwPWtXQ9O7EgnU</t>
+  </si>
+  <si>
+    <t>Harry Potter dan Batu Bertuah</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/0ekfK5UxfB3ang67AaJE2w</t>
+  </si>
+  <si>
+    <t>Olenka</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/1Yz8Mn7kAiqx6nSftlhoDl</t>
+  </si>
+  <si>
+    <t>Harimau! Harimau!</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/1oRJjHli3BBx4GDnxUb6H5</t>
+  </si>
+  <si>
+    <t>Man's Search for Meaning</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/0JIjvVKAlJLpjqAyOSz409</t>
+  </si>
+  <si>
+    <t>When Breath Becomes Air</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/0iZb9U0NGCexM0CtMaCLbY</t>
+  </si>
+  <si>
+    <t>Harry Potter dan Kamar Rahasia</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/7zu5Mt2HJSatqAWjaFWs1A</t>
+  </si>
+  <si>
+    <t>The Book of Ikigai</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/7hRN6nN1WudRC1tNvWkUZo</t>
+  </si>
+  <si>
+    <t>Bukan Pasar Malam</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/2Fu8N2YzbRSIxt2bHRQh2X</t>
+  </si>
+  <si>
+    <t>Hadji Dadjal</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/6r0LIKkmWnL9RzL7rzQtxe</t>
+  </si>
+  <si>
+    <t>Awal dan Mira</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/6loTs9RUMB1zanjDRDtiUg</t>
+  </si>
+  <si>
+    <t>Apakah Kamu Ibuku?</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/4r41cSn3nctzASQXAvzM1W</t>
+  </si>
+  <si>
+    <t>Animal Farm</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/embed/episode/3mnPjnyWiyg5ovluhFfDzC</t>
+  </si>
+  <si>
+    <t>goodreads_ratings_count</t>
+  </si>
+  <si>
+    <t>goodreads_link</t>
+  </si>
+  <si>
+    <t>Abdul Mun'im Idries</t>
+  </si>
+  <si>
+    <t>&lt;a class="Footer__badge" href="https://play.google.com/store/apps/details?id=com.goodreads&amp;amp;utm_source=mw_footer&amp;amp;pcampaignid=MKT-Other-global-all-co-prtnr-py-PartBadge-Mar2515-1"&gt;&lt;img alt="Download app for Android" data-nimg="1" decoding="async" height="40" loading="lazy" src="/_next/image?url=https%3A%2F%2Fdryofg8nmyqjw.cloudfront.net%2Fimages%2Fbadge-google_play_store%402x.png&amp;amp;w=384&amp;amp;q=75" srcset="/_next/image?url=https%3A%2F%2Fdryofg8nmyqjw.cloudfront.net%2Fimages%2Fbadge-google_play_store%402x.png&amp;amp;w=256&amp;amp;q=75 1x, /_next/image?url=https%3A%2F%2Fdryofg8nmyqjw.cloudfront.net%2Fimages%2Fbadge-google_play_store%402x.png&amp;amp;w=384&amp;amp;q=75 2x" style="color:transparent" width="135"/&gt;&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Crime, Mystery, Indonesian Literature, Nonfiction, History</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1370323544i/18038661.jpg</t>
+  </si>
+  <si>
+    <t>“Kamu gila. Ngelawan arus. Pulang tinggal nama entar." Begitu yang terlontar dari kolega dr. Abdul Mun’im Idries, ketika akhir 1993, dokter forensik ini berani menjadi saksi ahli kasus pembunuhan Marsinah. Kala itu, santer diyakini pejuang buruh ini dihabisi oknum militer—ketika militer paling ditakuti dengan penculikan senyapnya. Tapi berani-beraninya Mun’im mengusik tentara. Lalu, apa yang dihadapi Mun’im dan fakta apa yang ia temukan ketika harus terjun pada detik-detik mencekam Tragedi Trisakti dan Tragedi Semanggi? Bagaimana analisis forensiknya terkait pembunuhan Munir, Tragedi Tanjung Priuk, Tragedi Beutong Ateuh, dan sebagainya? Mun’im dalam buku ini membongkar arsip, membeberkan fakta-fakta mengejutkan, mengungkap sejumlah nama tabu, di samping berbagi kisah dan cara ilmiah (kedokteran) forensik dalam membongkar kriminalitas dan kejahatan di negeri ini.</t>
+  </si>
+  <si>
+    <t>Novels, Poetry, Fiction, Romance, Indonesian Literature</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1398848827i/22025401.jpg</t>
+  </si>
+  <si>
+    <t>Yang menulis di buku ini belum tentu saya, sebab Rahwana tak mati-mati. Gunung kembar Sondara-Sondari yang menghimpit Rahwana cuma mematikan tubuhnya semata. Jiwa Rahwana terus hidup. Hidupnya menjadi gelembung-gelembung. Siapa pun bisa dihinggapi gelembung itu tak terkecuali saya. Yang menulis di buku ini adalah gelembung-gelembung itu, gelembung Rahwana padaku. Yang menyampaikan buku ini padamu adalah gelembung-gelembung Rahwana pada penerbit, percetakan, distributor, toko buku dan lain-lain tak terkecuali tukang ojek yang mengantarmu ke toko buku maupun perpustakaan. Bila gelembung-gelembung Rahwana itu tak ada padamu, kau akan menolak pergi ke toko buku. Sekadar meminjam buku ini ke teman pun, kau tak akan berdaya bila gelembung-gelembung Rahwana tak menjangkitimu. Kau pun tak akan nge-twit dan sebagainya tentang buku ini. Bila gelembung-gelembung Rahwana tak menjangkitimu, tak ada alasan bagimu mengggunakan seluruh media sosial dan getok tular buat menjalarkan cinta via buku in...</t>
+  </si>
+  <si>
+    <t>Short Stories, Fiction, Romance, Russia, Russian Literature</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1234155794i/6063415.jpg</t>
+  </si>
+  <si>
+    <t>Diterjemahkan dari edisi bahasa Inggris A Happy Married Life terjemahan Margaret Wettlin.Cetakan kedua.Rumah Tangga yang Bahagia melukiskan percintaan antara seorang gadis dengan seorang lelaki yang jauh lebih tua. Dengan cermat digambarkan betapa halus pertumbuhan benih cinta dalam hati si gadis. Walaupun terpaksa menghadapi berbagai pertentangan dan kesalahpahaman, namun keagungan cintalah yang pada akhirnya berbuahkan kebahagiaan.</t>
+  </si>
+  <si>
+    <t>Ernest Hemingway</t>
+  </si>
+  <si>
+    <t>American, Novels, Literary Fiction, Fiction, School</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1243229870i/6493574.jpg</t>
+  </si>
+  <si>
+    <t>Novel memukau yang membangkitkan optimisme ini adalah karya terbaik Ernest Hemingway, pengarang legendaris Amerika dan pemenang Hadiah Nobel Sastra 1954, sekaligus novel terakhirnya yang terbit semasa hidupnya.Lelaki Tua dan Laut (The Old Man and the Sea) berkisah tentang perjuangan luar biasa seorang nelayan tua Kuba yang seorang diri berusaha menangkap ikan marlin raksasa jauh di laut lepas setelah sebelumnya gagal menangkap seekor ikan pun selama 84 hari dan persahabatannya dengan seorang anak lelaki. Perjuangan pantang menyerah sang lelaki tua dalam mencapai tujuannya mengajarkan kepada kita betapa kesabaran, ketabahan, dan kegigihan dalam mengarungi cobaan hidup tak akan berakhir sia-sia.Novel yang asyik dibaca ini ditulis Hemingway saat tinggal di Kuba dan berhasil menyabet Hadiah Pulitzer 1953 untuk kategori fiksi serta Award of Merit Medal for Novel dari American Academy of Letters, sekaligus mengantarkannya meraih Hadiah Nobel Sastra. Sedemikian populernya novel menyentuh i...</t>
+  </si>
+  <si>
+    <t>Antoine de Saint-Exupéry</t>
+  </si>
+  <si>
+    <t>Childrens, France, Fiction, Fantasy, Classics</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1324474962i/13272459.jpg</t>
+  </si>
+  <si>
+    <t>Pangeran Cilik termasuk buku yang paling banyak diterjemahkan di dunia. Konon pernah disadur ke dalam 230 bahasa asing. Buku ini memang luar biasa. Tampaknya seolah cerita anak-anak, tapi sebenarnya dinikmati dan direnungkan juga oleh orang dewasa. Lewat cerita seorang anak yang mengamati dunia dengan mata naif dan lugu, Saint-Exupéry menyentuh beberapa nilai dan pengalaman manusia yang paling dasar, seperti kekuasaan, tanggung jawab, dan cinta. Dongeng yang mengharukan sekaligus amat mendalam ini termasuk karya-karya agung sastra dunia yang tidak terlupakan.</t>
+  </si>
+  <si>
+    <t>J.K. Rowling</t>
+  </si>
+  <si>
+    <t>Childrens, Magic, Fiction, Audiobook, Fantasy</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1310298517i/1611537.jpg</t>
+  </si>
+  <si>
+    <t>HARRY POTTER belum pernah jadi bintang tim Quidditch, mencetak angka sambil terbang tinggi naik sapu. Dia tak tahu mantra sama sekali, belum pernah membantu menetaskan naga ataupun memakai Jubah Gaib yang bisa membuatnya tidak kelihatan.Selama ini dia hidup menderita bersama paman dan bibinya, serta Dudley, anak mereka yang gendut dan manja. Kamar Harry adalah lemari sempit di bawah tangga loteng, dan selama sebelas tahun, belum pernah sekali pun dia merayakan ulang tahun.Tetapi semua itu berubah dengan datangnya surat misterius yang dibawa oleh burung hantu. Surat yang mengundangnya datang ke tempat luar biasa, tempat yang tak terlupakan bagi Harry--dan siapa saja yang membaca kisahnya. Karena di tempat itu dia tak hanya menemukan teman, olahraga udara, dan sihir dalam segala hal, dari pelajaran sampai makanan, melainkan juga takdirnya untuk menjadi penyihir besar... kalau Harry berhasil selamat berhadapan dengan musuh bebuyutannya.</t>
+  </si>
+  <si>
+    <t>Budi Darma</t>
+  </si>
+  <si>
+    <t>Novels, Fiction, Contemporary, Romance, Indonesian Literature</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1212740000i/1722607.jpg</t>
+  </si>
+  <si>
+    <t>Dalam Olenka, kita dibawa dalam alam absurd penuh obsesi dan ketidakberdayaan: sebuah petualangan pikiran lebih dari perjalanan jasmani. Seorang pria bernama Fanton Drummond, yang kita tahu adalah jelmaan pengarangnya sendiri, digambarkan begitu terobsesi dengan Olenka, seniman perempuan yang keberadaannya menyerupai hantu berkelibat. Dalam perjalanan spiritual ini muncul satu per satu tokoh dengan nama-nama yang terdengar normal sekaligus ganjil: Wayne Newton suami Olenka, tormented writer yang hanya bisa menghamburkan uang dan popularitasnya, M.B. dan M.C., Galpin Danzig, James Gilpur.</t>
+  </si>
+  <si>
+    <t>Mochtar Lubis</t>
+  </si>
+  <si>
+    <t>Novels, Fiction, Drama, Indonesian Literature, Classics</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1377676472i/1455669.jpg</t>
+  </si>
+  <si>
+    <t>Harimau! Harimau! telah mendapat Hadiah Yayasan Buku Utama sebagai buku penulisan sastra terbaik tahun 1975.Buku ini dapat dibaca sebagai sebuah cerita petualangan di rimba raya oleh sekelompok pengumpul damar yang diburu oleh seekor harimau yang kelaparan. Berhari-hari mereka mencoba menyelamatkan diri mereka dan seorang demi seorang di antara mereka jatuh menjadi korban terkaman harimau.Di tingkat lain, juga terjadi petualangan dalam diri masing-masing anggota kelompok pengumpul damar ini. Di bawah tekanan ancaman harimau yang terus-menerus memburu mereka, dalam diri meraka masing-masing, yang mempertinggi pula kesadaran mereka tentang kekuatan dan kelemahan-kelemahan para anggota kelompok mereka yang lain.Di antara mereka malahan sampai pada kesadaran bahwa sebelum membunuh harimau yang memburu-buru mereka, tak kalah pentingnya ialah untuk membunuh terlebih dahulu harimau yang berada dalam setiap anak manusia.Buku ini telah diterjemahkan ke dalam bahasa Inggris, Belanda, Jerman, ...</t>
+  </si>
+  <si>
+    <t>Viktor E. Frankl</t>
+  </si>
+  <si>
+    <t>Psychology, Memoir, Self Help, Audiobook, Biography</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1535419394i/4069.jpg</t>
+  </si>
+  <si>
+    <t>Psychiatrist Viktor Frankl's memoir has riveted generations of readers with its descriptions of life in Nazi death camps and its lessons for spiritual survival. Based on his own experience and the stories of his patients, Frankl argues that we cannot avoid suffering but we can choose how to cope with it, find meaning in it, and move forward with renewed purpose. At the heart of his theory, known as logotherapy, is a conviction that the primary human drive is not pleasure but the pursuit of what we find meaningful. Man's Search for Meaning has become one of the most influential books in America; it continues to inspire us all to find significance in the very act of living.</t>
+  </si>
+  <si>
+    <t>Paul Kalanithi</t>
+  </si>
+  <si>
+    <t>Memoir, Audiobook, Biography, Book Club, Medicine</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1492677644i/25899336.jpg</t>
+  </si>
+  <si>
+    <t>For readers of Atul Gawande, Andrew Solomon, and Anne Lamott, a profoundly moving, exquisitely observed memoir by a young neurosurgeon faced with a terminal cancer diagnosis who attempts to answer the question 'What makes a life worth living?'At the age of thirty-six, on the verge of completing a decade's worth of training as a neurosurgeon, Paul Kalanithi was diagnosed with stage IV lung cancer. One day he was a doctor treating the dying, and the next he was a patient struggling to live. And just like that, the future he and his wife had imagined evaporated. When Breath Becomes Air chronicles Kalanithi's transformation from a naïve medical student "possessed," as he wrote, "by the question of what, given that all organisms die, makes a virtuous and meaningful life" into a neurosurgeon at Stanford working in the brain, the most critical place for human identity, and finally into a patient and new father confronting his own mortality. What makes life worth living in the face of death...</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1310300647i/1611602.jpg</t>
+  </si>
+  <si>
+    <t>HARRY POTTER sudah tidak tahan lagi melewati liburan musim panas bersama keluarga Dursley yang menyebalkan, dan dia ingin sekali bisa segera kembali ke Sekolah Sihir Hogwarts. Tetapi tiba-tiba muncul makhluk aneh bernama Dobby, yang melarangnya kembali ke sana. Malapetaka akan menimpa Harry kalau dia berani kembali ke Hogwarts.Dan malapetaka betul-betul terjadi. Karena pada tahun keduanya di Hogwarts muncul siksaan dan penderitaan baru, dalam wujud guru baru sok bernama Gilderoy Lockhart, hantu bernama Myrtle Merana yang menghantui toilet anak perempuan, dan perhatian tak diinginkan dari adik Ron Weasley Ginny.Tetapi semua itu cuma gangguan kecil dibandingkan dengan bencana besar yang kemudian melanda sekolah: Ada yang mengubah murid-murid Hogwarts menjadi batu. Mungkinkah pelakunya Draco Malfoy yang jahat, pesaing utama Harry? Mungkinkah dia Hagrid, yang riwayat masa lalunya akhirnya terbongkat? Atau, mungkinkah pelakunya anak yang paling dicurigai semua orang di Hogwarts... yakni ...</t>
+  </si>
+  <si>
+    <t>Ken Mogi</t>
+  </si>
+  <si>
+    <t>Japan, Philosophy, Personal Development, Self Help, Audiobook</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1502463403i/36001608.jpg</t>
+  </si>
+  <si>
+    <t>'FORGET HYGGE. IT'S ALL ABOUT IKIGAI (THAT'S JAPANESE FOR A HAPPY LIFE)' The Times Find out how to live a long and happy life thanks to the ikigai miracle, a Japanese philosophy that helps you find fulfilment, joy and mindfulness in everything you do. It is extraordinary that Japanese men's longevity ranks 4th in the world, while Japanese women's ranks 2nd. But perhaps this comes as no surprise when you know that the Japanese understanding of ikigai is embedded in their daily life and in absolutely everything that they do. In their professional careers, in their relationships with family members, in the hobbies they cultivate so meticulously. Ken Mogi identifies five key pillars to ikigai:Pillar 1: Starting smallPillar 2: Releasing yourselfPillar 3:Harmony and sustainabilityPillar 4:The joy of little thingsPillar 5:Being in the here and nowThe Japanese talk about ikigai as 'a reason to get up in the morning'. It is something that keeps one's enthusiasm for life going, whether you ar...</t>
+  </si>
+  <si>
+    <t>Pramoedya Ananta Toer</t>
+  </si>
+  <si>
+    <t>Novels, Fiction, Historical Fiction, Drama, Indonesian Literature</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1369464565i/1670518.jpg</t>
+  </si>
+  <si>
+    <t>Perjalanan seorang anak revolusi yang pulang kampung karena ayahandanya jatuh sakit. Dari seputaran perjalanan itu, terungkap beberapa potong puing gejolak hati yang teka pernah teranggap dalam gebyar-gebyar revolusi.Dikisahkan bagaimana keperwiraan seseorang dalam revolusi pada akhirnya melunak ketika dihadapkan pada kenyataan sehari-hari: ia menemukan ayahnya yang seorang guru yang penuh bakti tergolek sakit karena TBC, anggota keluarganya yang miskin, rumah tuanya yang sudah tidak kuat lagi menahan arus waktu, dan menghadapi istri yang cerewet.Berpotong-potong kisah itu diungkapkan dengan sisa-sisa kekuatan jiwa yang berenangan dalam jiwa seorang mantan tentara muda revolusi yang idealis. Lewat tuturan yang sederhana dan fokus, tokoh "aku" dalam roman ini tidak hanya mengritik kekerdilan diri sendiri, tapi juga menunjuk muka para jendral atau pembesar negeri paskakemerdekaan yang hanya asyik mengurus dan memperkaya diri sendiri.</t>
+  </si>
+  <si>
+    <t>Utuy Tatang Sontani</t>
+  </si>
+  <si>
+    <t>Drama, Indonesian Literature, Fiction</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1349405930i/16067931.jpg</t>
+  </si>
+  <si>
+    <t>Sebuah novel roman yang menceritakan kehidupan manusia2 yang cacat akibat perang revolusi sehingga menjadi badut hinaan manusia2 lain yang tak ikut berperang tapi mendapatkan keuntungan lebih banyak. Mengisahkan tentang perjuangan seorang pemuda bernama Awal untuk merebut cinta Mira seorang gadis cantik pemilik kedai kopi yang cacat fisik akibat perang revolusi. Karya Utuy ini pernah mendapat penghargaan dari B.M.K.N sebagai naskah drama terbaik di tahun 1952."Kan didjaman sekarang ini banjak padukatuan jang didjaman peperangan pada bersembunji takut mati, tiba-tiba sekarang muntjul dengan kedudukannja jang hebat-hebat, sangking hebatnja merasa perlu mempunjai bini dua tiga"(AWAL &amp; MIRA, halaman 17)</t>
+  </si>
+  <si>
+    <t>George Orwell</t>
+  </si>
+  <si>
+    <t>Novels, Science Fiction, Dystopia, Fiction, School</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1325861570i/170448.jpg</t>
+  </si>
+  <si>
+    <t>Librarian's note: There is an Alternate Cover Edition for this edition of this book here.A farm is taken over by its overworked, mistreated animals. With flaming idealism and stirring slogans, they set out to create a paradise of progress, justice, and equality. Thus the stage is set for one of the most telling satiric fables ever penned –a razor-edged fairy tale for grown-ups that records the evolution from revolution against tyranny to a totalitarianism just as terrible. When Animal Farm was first published, Stalinist Russia was seen as its target. Today it is devastatingly clear that wherever and whenever freedom is attacked, under whatever banner, the cutting clarity and savage comedy of George Orwell’s masterpiece have a meaning and message still ferociously fresh.</t>
+  </si>
+  <si>
+    <t>DAFTAR ISI
+00:00:00 INTRO
+00:00:09 BAGIAN 1
+00:00:13 TIGA ANAK JEMBEL
+00:07:10 WAYNE DAN STEVEN
+00:15:58 OLENKA DALAM CERITA
+00:22:06 DALAM BAYANGAN OLENKA
+00:32:38 BERTEMU DENGAN OLENKA
+00:39:47 PERTEMUAN-PERTEMUAN SELANJUTNYA
+00:45:31 THE NEW ENGLAND MIND
+00:48:05 MENARA LONCENG ELBERHART
+00:52:48 OLENKA MENELEPON
+00:57:45 CARA MENULIS WAYNE
+01:06:14 KUTU
+01:17:47 OLENKA MENINGGALKAN SAYA
+01:29:30 OLENKA MENURUT WAYNE
+01:41:00 OLENKA BERKELEBAT LAGI
+01:44:31 MARILAH KITA MILIKI SATU DUNIA
+01:48:04 SAYA MENGINGINKAN ANAK
+01:53:16 CEMBURU
+02:02:32 BISU
+02:06:03 MENGEMBARA KE KENTUCKY
+02:14:47 TIGA SURAT WAYNE
+02:22:27 WAYNE SUDAH KELUAR
+02:31:20 MUSIM DAN CACING
+02:43:36 SAYA MENGHAJAR WAYNE
+02:48:22 BAGIAN 2
+02:48:26 JANE PENGGANTI OLENKA
+02:52:10 MELAWAT KE CHICAGO
+03:01:39 PINANGAN
+03:09:46 MC PULANG SENDIRIAN
+03:17:49 SEMALAM DI INDIANAPOLIS
+03:37:38 WAYNE GALPIN DAN SAYA
+03:40:10 BAGIAN 3
+03:40:14 LIMA SURAT MASTURBASI
+03:54:19 MUSIBAH
+03:58:37 MADAME SOSOSTRIS
+04:12:18 MIMPI
+04:18:37 BAGIAN 4
+04:18:41 SURAT PANJANG OLENKA
+05:09:29 SURAT SEORANG PEMBACA
+05:12:33 KELANJUTAN SURAT OLENKA
+05:17:54 TERBANG
+05:27:57 SURAT KILAT KHUSUS
+05:33:43 ALIQUIPPA
+05:38:10 BERTEMU KEMBALI DENGAN MC
+05:49:51 PINANGAN KEDUA
+05:59:45 COTTAGE
+06:10:53 BIARLAH USIA BERSEKONGKOL DENGAN MASA MUDA
+06:18:52 MENINGGALKAN MC
+06:28:13 NAUSEA
+06:43:03 BAGIAN 5
+06:43:07 CODA
+06:46:20 BAGIAN 6
+06:46:24 ASAL-USUL OLENKA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2F1DnzcmRg2b1K1ExJGRwS  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3rja5LL0jTl2QmDgrwNbjo  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4wujUHwiQ4UeZmhUNk7H4J  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">719qnUT6Zm6m7IzQbbf4OO  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">31c7kpXIOJUj7k8wcL8RMP  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2EK3MJF4bwPWtXQ9O7EgnU  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0ekfK5UxfB3ang67AaJE2w  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1Yz8Mn7kAiqx6nSftlhoDl  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1oRJjHli3BBx4GDnxUb6H5  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0JIjvVKAlJLpjqAyOSz409  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0iZb9U0NGCexM0CtMaCLbY  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7zu5Mt2HJSatqAWjaFWs1A  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7hRN6nN1WudRC1tNvWkUZo  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2Fu8N2YzbRSIxt2bHRQh2X  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6r0LIKkmWnL9RzL7rzQtxe  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6loTs9RUMB1zanjDRDtiUg  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4r41cSn3nctzASQXAvzM1W  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3mnPjnyWiyg5ovluhFfDzC  </t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Gadis</t>
+  </si>
+  <si>
+    <t>Ardi</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Daftar Isi
+00:00:00 Bab 1 Menyibak Fakta-Fakta Tersembunyi
+00:00:08 Trisakti Mei 1998
+00:14:43 Misteri Kasus Semanggi
+00:23:48 Kejanggalan Kematian Marsinah
+00:31:26 Tragedi Tanjung Priok
+00:37:06 Misteri Kematian Sang Proklamator
+00:45:15 Tjetje dan Kasus Kematian dalam Tahanan
+00:49:32 Mengungkap Narkoba di Balik Kematian Aldi
+00:55:40 Misteri Kematian De Guzman
+00:59:56 Mayat Siapa
+01:03:22 Nasrudin Menguak Cerita yang Disamarkan
+01:18:04 Bab 2 KasusKasus Kedokteran Forensik Serangkaian Kisah Membongkar Kejahatan
+01:18:13 30 Menit Kematian Menjemput Munir
+01:36:54 Saat Bedah Mayat Mengungkap Kebenaran
+01:45:57 Saat Penggalian Mayat Mengungkap Fakta
+01:50:03 Kasus Surat Keterangan Dokter
+01:54:14 Saat Cairan Sperma Bicara
+02:03:10 Otopsi Bedah Mayat dalam Kasus Pembunuhan
+02:08:37 Mati Ditembak atau Karena Ledakan Mobil
+02:15:20 Bedah Mayat Untuk Kecelakaan Pesawat
+02:21:29 Malpraktik
+02:26:47 Saksi Atas Kematian Udin
+02:32:39 Memastikan Tersangka Penembak Zaenuddin
+02:37:53 Menyingkap Tragedi Beutong Ateuh
+02:43:51 Bab 3 Mengungkap Kejahatan Narkoba
+02:43:57 Minuman Keras dan Kriminalitas
+02:49:05 Psikotropika
+02:53:46 Ekstasi dan Zarina
+03:00:31 Menjaring Pengguna Ekstasi
+03:06:43 Aspek Forensik dari Alkohol
+03:14:27 Bab 4 Membongkar kekerasan Seksual dan Kejahatan Terhadap Anak
+03:14:34 Perlakuan Salah terhadap Anak
+03:20:37 Profil Pembantai Anak Jalanan Memburu Robot Gedek 2
+03:28:07 Awas Pedofilia di Sekitar Kita
+03:32:58 Kasus Menjual Keperawanan
+03:37:40 Kasus Bayi Tertukar
+03:42:25 BayiBayi yang Malang
+03:46:54 Aborsi Kejahatan Tanpa Korban
+03:53:06 Bab 5 Kedokteran Forensik Sebagai Pisau Ilmiah
+03:53:14 Kedokteran Forensik Upaya Ilmiah untuk Penegakan Hukum dan Keadilan
+04:04:39 Masyarakat Berhak Tahu Hasil Visum
+04:11:54 Kapan Seseorang Dinyatakan Sudah Meninggal Dunia
+04:22:13 Segi Forensik dari Kematian Mendadak
+04:30:22 Cara Identifikasi Massal Korban Kerusuhan
+04:37:53 Identifikasi Massal dan Korban Kebakaran
+04:43:59 Bab 6 Pembunuhan Sadis Amukan Massa dan Kematian Tokoh
+04:44:07 Kasus Mayat Terpotong 13
+04:46:21 Membuka Lembaran Lama Marsinah
+04:51:11 Teror Terhadap Jubah Hakim
+04:59:56 Memancing Amarah Papua
+05:08:07 Hercules
+05:10:48 Faturrahman alGhozi</t>
+  </si>
+  <si>
+    <t>Daftar Isi
+00:00:00 Intro
+00:00:10 Teratai
+00:09:50 Berlin
+00:28:18 Swan
+00:44:38 Lokapala
+01:05:32 Kundalini I
+01:20:47 Napas
+01:33:58 Lumba-Lumba
+01:47:23 Tukang Sayur
+02:08:34 Prenjak
+02:28:45 LayangLayang
+02:29:14 Dawet Ayu
+02:54:19 Sinta
+03:15:28 Kundalini II
+03:18:22 Mandodari
+03:26:51 Sastrajendra
+03:46:37 Mata Sapi
+04:10:58 Cokelat
+04:29:27 Gantal
+04:40:33 Dardanella
+04:49:49 Soliloquy</t>
+  </si>
+  <si>
+    <t>DAFTAR ISI
+00:00:00 INTRO
+00:00:10 BAGIAN PERTAMA
+00:00:15 Bab Satu
+00:19:58 Bab Dua
+00:48:36 Bab Tiga
+01:22:34 Bab Empat
+01:48:56 Bab Lima
+02:15:40 BAGIAN KEDUA
+02:15:44 Bab Enam
+02:52:52 Bab Tujuh
+03:25:04 Bab Delapan
+03:56:08 Bab Sembilan</t>
+  </si>
+  <si>
+    <t>Daftar Isi
+00:00:00 Intro
+00:00:07 1
+00:02:55 2
+00:07:22 3
+00:09:59 4
+00:14:47 5
+00:18:47 6
+00:20:09 7
+00:24:39 8
+00:28:48 9
+00:31:35 10
+00:39:10 11
+00:41:02 12
+00:41:58 13
+00:47:31 14
+00:51:42 15
+00:56:47 16
+00:58:16 17
+01:01:33 18
+01:02:24 19
+01:03:33 20
+01:05:00 21
+01:13:12 22
+01:14:49 23
+01:15:36 24
+01:19:23 25
+01:23:58 26
+01:32:41 27</t>
+  </si>
+  <si>
+    <t>Daftar Isi
+00:00:00 Intro
+00:00:10 1. Anak Laki-laki Yang Bertahan Hidup
+00:30:25 2. Kaca Yang Lenyap
+00:51:37 3. Surat Dari Entah Siapa
+01:16:08 4. Si Pemegang Kunci
+01:40:48 5. Diagon Alley
+02:26:36 6. Perjalanan Dari Peron Sembilan Tiga Perempat
+03:09:22 7. Topi Seleksi
+03:40:25 8. Ahli Ramuan
+04:00:53 9. Duel Tengah Malam
+04:35:11 10. Halloween
+05:04:00 11. Quidditch
+05:26:12 12. Cermin Tarsah
+06:03:14 13. Nicolas Flamel
+06:25:17 14. Norbert Si Naga Punggung Bersirip Norwegia
+06:48:16 15. Hutan Terlarang
+07:22:42 16. Menembus Pintu Jebakan Di tahun-tahun mendatang
+08:06:38 17. Laki-laki Dengan Dua Wajah</t>
+  </si>
+  <si>
+    <t>Daftar Isi
+00:00:00 Intro
+00:00:09 Prolog
+00:00:51 1
+00:09:08 2
+01:17:20 3
+01:58:18 4
+02:48:05 5
+03:18:34 6
+04:04:33 7</t>
+  </si>
+  <si>
+    <t>Daftar Isi
+00:00:00 Mencari Makna Hidup - Sebuah Pengantar
+00:06:51 Kebahagiaan dan Kesuksesan Tidak Dapat Dikejar - Pengantar Edisi 1992
+00:13:14 01 - Pengalaman di Kamp Konsentrasi
+03:06:18 02 - Logoterapi Secara Ringkas
+04:13:03 Catatan Akhir 1984
+04:13:09 Optimisme Di Tengah Tragedi
+04:42:55 Penutup</t>
+  </si>
+  <si>
+    <t>Daftar Isi
+00:00:00 Intro
+00:00:49 Prolog
+00:19:33 Bagian 1
+02:30:16 Bagian 2
+04:21:24 Epilog</t>
+  </si>
+  <si>
+    <t>Daftar Isi
+00:00:00 Intro
+00:00:10 1. Ulang Tahun Paling Buruk
+00:16:49 2. Peringatan Dobby
+00:36:24 3. The Burrow
+01:05:18 4. Di Flourish And Blotts
+01:42:15 5. Dedalu Perkasa
+02:18:26 6. Gilderoy Lockhart
+02:49:31 7. DarahLumpur Dan Bisikan-Bisikan
+03:19:59 8. Hari Ulang Tahun Kematian
+03:49:13 9. Tulisan Di Dinding
+04:23:44 10. Bludger Gila
+04:58:59 11. Klub Duel
+05:40:08 12. Ramuan Polijus
+06:15:54 13. Buku Harian Yang Sangat Rahasia
+06:52:05 14. Cornelius Fudge
+07:18:51 15. Aragog
+07:49:02 16. Kamar Rahasia
+08:27:40 17. Pewaris Slytherin
+09:05:55 18. Pahala Untuk Dobby</t>
+  </si>
+  <si>
+    <t>DAFTAR ISI
+00:00:00 INTRO
+00:00:14 CATATAN - Lima Pilar Ikigai
+00:01:27 BAB 1 - Arti Ikigai
+00:20:47 BAB 2 - Alasan Anda Bangun Pagi
+00:38:51 BAB 3 - Keindahan Indriawi Ikigai
+01:05:03 BAB 4 - Keindahan Indriawi Ikigai
+01:20:58 BAB 5 - Aliran dan Kreativitas
+01:47:04 BAB 6 - Ikigai dan Kelestarian
+02:07:27 BAB 7 - Menemukan Makna Hidup Anda
+02:36:36 BAB 8 - Yang Tidak Membunuhmu akan Menjadikanmu Lebih Kuat
+02:54:03 BAB 9 - Ikigai dan Kebahagiaan
+03:12:22 BAB 10 - Terima Diri Anda Apa Adanya
+03:22:52 KESIMPULAN - Temukan Ikigai Anda Sendiri</t>
+  </si>
+  <si>
+    <t>Daftar Isi
+00:00:00 Intro
+00:00:10 1
+00:06:01 2
+00:18:41 3
+00:23:46 4
+00:32:40 5
+00:42:01 6
+00:48:34 7
+00:59:06 8
+01:09:52 9
+01:35:48 10
+01:38:47 11
+01:46:53 12
+01:51:40 13
+02:01:26 14
+02:10:46 15
+02:13:57 16</t>
+  </si>
+  <si>
+    <t>DAFTAR ISI
+00:00:00 INTRO
+00:00:09 BAGIAN 1
+00:09:29 BAGIAN 2
+00:23:18 BAGIAN 3
+00:36:18 BAGIAN 4
+00:50:30 BAGIAN 5
+00:58:47 BAGIAN 6
+01:09:01 BAGIAN 7
+01:15:47 BAGIAN 8</t>
+  </si>
+  <si>
+    <t>Daftar Isi
+00:00:00 Intro
+00:00:09 Bab 1
+00:16:29 Bab 2
+00:30:45 Bab 3
+00:44:33 Bab 4
+00:55:04 Bab 5
+01:14:14 Bab 6
+01:32:39 Bab 7
+01:54:30 Bab 8
+02:19:00 Bab 9
+02:42:04 Bab 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3062,12 +3754,34 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF98C379"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3102,17 +3816,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipertaut" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4551,14 +5288,927 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8285C9E-72DA-48D1-A913-B6476B42EC48}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>1129</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="L1" t="s">
+        <v>998</v>
+      </c>
+      <c r="M1" t="s">
+        <v>247</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.22424768518518517</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1014</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>1111</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>1133</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1053</v>
+      </c>
+      <c r="I2">
+        <v>3.97</v>
+      </c>
+      <c r="J2">
+        <v>532</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1055</v>
+      </c>
+      <c r="M2">
+        <v>2013</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1056</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="330" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.20548611111111112</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>1017</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>1112</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>1134</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1016</v>
+      </c>
+      <c r="I3">
+        <v>4.07</v>
+      </c>
+      <c r="J3" s="6">
+        <v>1091</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1058</v>
+      </c>
+      <c r="M3">
+        <v>2014</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1059</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="195" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.18782407407407409</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>1113</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>1135</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1019</v>
+      </c>
+      <c r="I4">
+        <v>3.91</v>
+      </c>
+      <c r="J4" s="6">
+        <v>13448</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1061</v>
+      </c>
+      <c r="M4">
+        <v>1859</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1062</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C5" s="5">
+        <v>7.1805555555555553E-2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>1114</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I5">
+        <v>3.81</v>
+      </c>
+      <c r="J5">
+        <v>1239112</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1065</v>
+      </c>
+      <c r="M5">
+        <v>1952</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1066</v>
+      </c>
+      <c r="O5" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C6" s="5">
+        <v>6.4120370370370373E-3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>1024</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>1115</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C7" s="5">
+        <v>6.626157407407407E-2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>1026</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>1116</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1068</v>
+      </c>
+      <c r="I7">
+        <v>4.33</v>
+      </c>
+      <c r="J7">
+        <v>2310739</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1069</v>
+      </c>
+      <c r="M7">
+        <v>1943</v>
+      </c>
+      <c r="N7" t="s">
+        <v>1070</v>
+      </c>
+      <c r="O7" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="285" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.3643865740740741</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>1117</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>1137</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1072</v>
+      </c>
+      <c r="I8">
+        <v>4.47</v>
+      </c>
+      <c r="J8">
+        <v>10859746</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1073</v>
+      </c>
+      <c r="M8">
+        <v>1997</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1074</v>
+      </c>
+      <c r="O8" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.29594907407407406</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>1110</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1076</v>
+      </c>
+      <c r="I9">
+        <v>3.99</v>
+      </c>
+      <c r="J9">
+        <v>1149</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1077</v>
+      </c>
+      <c r="M9">
+        <v>1983</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1078</v>
+      </c>
+      <c r="O9" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="150" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.21138888888888888</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>1119</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>1138</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1080</v>
+      </c>
+      <c r="I10">
+        <v>4.08</v>
+      </c>
+      <c r="J10">
+        <v>3016</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1081</v>
+      </c>
+      <c r="M10">
+        <v>1975</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1082</v>
+      </c>
+      <c r="O10" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="165" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.21089120370370371</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>1139</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1084</v>
+      </c>
+      <c r="I11">
+        <v>4.37</v>
+      </c>
+      <c r="J11">
+        <v>805682</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1085</v>
+      </c>
+      <c r="M11">
+        <v>1946</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1086</v>
+      </c>
+      <c r="O11" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.20443287037037036</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>1036</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1088</v>
+      </c>
+      <c r="I12">
+        <v>4.41</v>
+      </c>
+      <c r="J12">
+        <v>745217</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1089</v>
+      </c>
+      <c r="M12">
+        <v>2016</v>
+      </c>
+      <c r="N12" t="s">
+        <v>1090</v>
+      </c>
+      <c r="O12" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="330" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.39776620370370369</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>1122</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1072</v>
+      </c>
+      <c r="I13">
+        <v>4.43</v>
+      </c>
+      <c r="J13">
+        <v>4265150</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1073</v>
+      </c>
+      <c r="M13">
+        <v>1998</v>
+      </c>
+      <c r="N13" t="s">
+        <v>1092</v>
+      </c>
+      <c r="O13" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="270" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.14346064814814816</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>1123</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>1142</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1094</v>
+      </c>
+      <c r="I14">
+        <v>3.58</v>
+      </c>
+      <c r="J14">
+        <v>15148</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1095</v>
+      </c>
+      <c r="M14">
+        <v>2017</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1096</v>
+      </c>
+      <c r="O14" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="270" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C15" s="5">
+        <v>9.6157407407407414E-2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>1042</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>1124</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>1143</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1098</v>
+      </c>
+      <c r="I15">
+        <v>4.05</v>
+      </c>
+      <c r="J15">
+        <v>2518</v>
+      </c>
+      <c r="K15" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L15" t="s">
+        <v>1099</v>
+      </c>
+      <c r="M15">
+        <v>1950</v>
+      </c>
+      <c r="N15" t="s">
+        <v>1100</v>
+      </c>
+      <c r="O15" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="150" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C16" s="5">
+        <v>6.4351851851851855E-2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>1125</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>1144</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C17" s="5">
+        <v>3.9166666666666669E-2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G17" s="11"/>
+      <c r="H17" t="s">
+        <v>1102</v>
+      </c>
+      <c r="I17">
+        <v>3.89</v>
+      </c>
+      <c r="J17">
+        <v>73</v>
+      </c>
+      <c r="K17" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L17" t="s">
+        <v>1103</v>
+      </c>
+      <c r="M17">
+        <v>1952</v>
+      </c>
+      <c r="N17" t="s">
+        <v>1104</v>
+      </c>
+      <c r="O17" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C18" s="5">
+        <v>5.3935185185185188E-3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>1048</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="180" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.12708333333333333</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>1050</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>1128</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>1145</v>
+      </c>
+      <c r="H19" t="s">
+        <v>1106</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19">
+        <v>4242426</v>
+      </c>
+      <c r="K19" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L19" t="s">
+        <v>1107</v>
+      </c>
+      <c r="M19">
+        <v>1945</v>
+      </c>
+      <c r="N19" t="s">
+        <v>1108</v>
+      </c>
+      <c r="O19" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{BA76D9C0-BE4F-457D-BBDD-8BDAFEE4BB8F}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{8DAFC59E-9FD6-4EA9-957A-45A0B0E28AE4}"/>
+    <hyperlink ref="E19" r:id="rId3" xr:uid="{E19D64A1-1F70-4A9A-88F6-B08F70197FC6}"/>
+    <hyperlink ref="E18" r:id="rId4" xr:uid="{4F97ABC5-26A4-4BD2-A194-E5CA3E2DFF21}"/>
+    <hyperlink ref="E17" r:id="rId5" xr:uid="{A84FC52B-A161-49BF-96C8-0B6246EACE6C}"/>
+    <hyperlink ref="E16" r:id="rId6" xr:uid="{C0D4F064-54ED-4C10-BDD1-A847EB9C41FF}"/>
+    <hyperlink ref="E15" r:id="rId7" xr:uid="{D12CB5D5-AE25-4417-A2A3-A499FC44206D}"/>
+    <hyperlink ref="E14" r:id="rId8" xr:uid="{3AF0329D-BA28-43AD-BDD4-7E46DD1FD775}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{12B67DEF-32D1-46F6-85BD-6A5CBC93A87E}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{7CCFFA31-1221-4390-8C58-16F6B43DD77B}"/>
+    <hyperlink ref="E10" r:id="rId11" xr:uid="{7F62FDC5-872C-449F-B37D-2B04C7A919D7}"/>
+    <hyperlink ref="E9" r:id="rId12" xr:uid="{0BAD0B6B-9018-48C7-B421-9C4700591A12}"/>
+    <hyperlink ref="E6" r:id="rId13" xr:uid="{3E51C248-A1FB-4489-8FDF-0B8700E42AD7}"/>
+    <hyperlink ref="E5" r:id="rId14" xr:uid="{798761FD-15A5-45CE-90E0-4B8257BD2F19}"/>
+    <hyperlink ref="E4" r:id="rId15" xr:uid="{B62A6749-E2B6-400D-A051-AB2A3E805D34}"/>
+    <hyperlink ref="E7" r:id="rId16" xr:uid="{9E393471-C286-4DFC-88FF-5D79ED665B53}"/>
+    <hyperlink ref="E13" r:id="rId17" xr:uid="{7794B149-FFDD-4C77-80B9-384309D05EF5}"/>
+    <hyperlink ref="E8" r:id="rId18" xr:uid="{1F9073A7-029F-4B6F-A2C5-FBDD03F28845}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4567,8 +6217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC66"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1:AC2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8852,7 +10502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82C0F13-1631-4B7F-8AC8-D69C12136FE9}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>